<commit_message>
Update input Excel file for timeslices
</commit_message>
<xml_diff>
--- a/scenario work/China/data/input_data_48_CHN.xlsx
+++ b/scenario work/China/data/input_data_48_CHN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zakeri\Documents\Github\time_clustering\scenario work\China\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A7941D-0B81-4CBE-AF67-7F79D3E5FDEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F77BD04F-1BDF-4FE1-B381-11984F2F5C66}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{821295F0-1D2B-4139-A10C-48DD9AE81549}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="12600" activeTab="1" xr2:uid="{821295F0-1D2B-4139-A10C-48DD9AE81549}"/>
   </bookViews>
   <sheets>
     <sheet name="time_steps" sheetId="3" r:id="rId1"/>
@@ -418,7 +418,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -470,12 +470,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -2020,7 +2014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D8AE0E0-9791-4693-801D-CFB5F73C4085}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
@@ -2989,8 +2983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C914A117-CEB2-443F-B651-C665C023F93B}">
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="I81" sqref="I81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3970,10 +3964,10 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B66" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C66" s="6" t="s">
         <v>23</v>
@@ -3985,10 +3979,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B67" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C67" s="6" t="s">
         <v>24</v>
@@ -4000,10 +3994,10 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B68" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>25</v>
@@ -4015,10 +4009,10 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B69" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C69" s="6" t="s">
         <v>26</v>
@@ -4030,10 +4024,10 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B70" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C70" s="6" t="s">
         <v>27</v>
@@ -4045,10 +4039,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B71" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C71" s="6" t="s">
         <v>28</v>
@@ -4060,10 +4054,10 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B72" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C72" s="6" t="s">
         <v>29</v>
@@ -4075,10 +4069,10 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B73" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C73" s="6" t="s">
         <v>30</v>
@@ -4090,10 +4084,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B74" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C74" s="6" t="s">
         <v>31</v>
@@ -4105,10 +4099,10 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B75" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C75" s="6" t="s">
         <v>32</v>
@@ -4120,10 +4114,10 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B76" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>33</v>
@@ -4135,10 +4129,10 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B77" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C77" s="6" t="s">
         <v>34</v>
@@ -4150,10 +4144,10 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B78" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C78" s="6" t="s">
         <v>35</v>
@@ -4165,10 +4159,10 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B79" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C79" s="6" t="s">
         <v>36</v>
@@ -4180,10 +4174,10 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B80" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C80" s="6" t="s">
         <v>37</v>
@@ -4195,10 +4189,10 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B81" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C81" s="6" t="s">
         <v>38</v>
@@ -4210,10 +4204,10 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C82" s="6" t="s">
         <v>39</v>
@@ -4225,10 +4219,10 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C83" s="6" t="s">
         <v>40</v>
@@ -4240,10 +4234,10 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B84" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C84" s="6" t="s">
         <v>41</v>
@@ -4255,10 +4249,10 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B85" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C85" s="6" t="s">
         <v>42</v>
@@ -4270,10 +4264,10 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B86" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C86" s="6" t="s">
         <v>43</v>
@@ -4285,10 +4279,10 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B87" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C87" s="6" t="s">
         <v>44</v>
@@ -4300,10 +4294,10 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B88" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C88" s="6" t="s">
         <v>45</v>
@@ -4315,10 +4309,10 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B89" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C89" s="6" t="s">
         <v>46</v>

</xml_diff>